<commit_message>
Added networking confs, fixed hanging threads bug
</commit_message>
<xml_diff>
--- a/transitions_to_real_P.xlsx
+++ b/transitions_to_real_P.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BroadcastSimulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ingframin/BroadcastSimulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47734252-2C26-354D-98AB-9B144CADDF4B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -56,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
@@ -461,27 +470,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="3.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="28.83203125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="3.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="3.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -509,7 +518,7 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>60</v>
       </c>
@@ -523,23 +532,23 @@
         <v>0.97297297297297303</v>
       </c>
       <c r="G2" s="8">
-        <f>C2*$A$2/(C2*$A$2+E2*$A$4+D2*$A$6)</f>
+        <f t="shared" ref="G2:G10" si="0">C2*$A$2/(C2*$A$2+E2*$A$4+D2*$A$6)</f>
         <v>9.9999999999999922E-2</v>
       </c>
       <c r="H2" s="8">
-        <f>D2*$A$6/(E2*$A$2+D2*$A$4+D2*$A$6)</f>
+        <f t="shared" ref="H2:H10" si="1">D2*$A$6/(E2*$A$2+D2*$A$4+D2*$A$6)</f>
         <v>0</v>
       </c>
       <c r="I2" s="8">
-        <f>E2*$A$4/(C2*$A$2+E2*$A$4+D2*$A$6)</f>
+        <f t="shared" ref="I2:I10" si="2">E2*$A$4/(C2*$A$2+E2*$A$4+D2*$A$6)</f>
         <v>0.90000000000000013</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K10" si="0">SUM(G2:I2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" ref="K2:K10" si="3">SUM(G2:I2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -553,23 +562,23 @@
         <v>0.94117647058823495</v>
       </c>
       <c r="G3" s="8">
-        <f>C3*$A$2/(C3*$A$2+E3*$A$4+D3*$A$6)</f>
+        <f t="shared" si="0"/>
         <v>0.20000000000000087</v>
       </c>
       <c r="H3" s="8">
-        <f>D3*$A$6/(E3*$A$2+D3*$A$4+D3*$A$6)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I3" s="8">
-        <f>E3*$A$4/(C3*$A$2+E3*$A$4+D3*$A$6)</f>
+        <f t="shared" si="2"/>
         <v>0.79999999999999916</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>15</v>
       </c>
@@ -583,23 +592,23 @@
         <v>0.90322580645161299</v>
       </c>
       <c r="G4" s="8">
-        <f>C4*$A$2/(C4*$A$2+E4*$A$4+D4*$A$6)</f>
+        <f t="shared" si="0"/>
         <v>0.29999999999999971</v>
       </c>
       <c r="H4" s="8">
-        <f>D4*$A$6/(E4*$A$2+D4*$A$4+D4*$A$6)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I4" s="8">
-        <f>E4*$A$4/(C4*$A$2+E4*$A$4+D4*$A$6)</f>
+        <f t="shared" si="2"/>
         <v>0.70000000000000018</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -613,23 +622,23 @@
         <v>0.85714285714285698</v>
       </c>
       <c r="G5" s="8">
-        <f>C5*$A$2/(C5*$A$2+E5*$A$4+D5*$A$6)</f>
+        <f t="shared" si="0"/>
         <v>0.4000000000000003</v>
       </c>
       <c r="H5" s="8">
-        <f>D5*$A$6/(E5*$A$2+D5*$A$4+D5*$A$6)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I5" s="8">
-        <f>E5*$A$4/(C5*$A$2+E5*$A$4+D5*$A$6)</f>
+        <f t="shared" si="2"/>
         <v>0.59999999999999976</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>100</v>
       </c>
@@ -644,23 +653,23 @@
         <v>0.8</v>
       </c>
       <c r="G6" s="8">
-        <f>C6*$A$2/(C6*$A$2+E6*$A$4+D6*$A$6)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="H6" s="8">
-        <f>D6*$A$6/(E6*$A$2+D6*$A$4+D6*$A$6)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I6" s="8">
-        <f>E6*$A$4/(C6*$A$2+E6*$A$4+D6*$A$6)</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C7" s="8">
         <v>0.27272727272727298</v>
       </c>
@@ -671,23 +680,23 @@
         <v>0.72727272727272696</v>
       </c>
       <c r="G7" s="8">
-        <f>C7*$A$2/(C7*$A$2+E7*$A$4+D7*$A$6)</f>
+        <f t="shared" si="0"/>
         <v>0.60000000000000031</v>
       </c>
       <c r="H7" s="8">
-        <f>D7*$A$6/(E7*$A$2+D7*$A$4+D7*$A$6)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I7" s="8">
-        <f>E7*$A$4/(C7*$A$2+E7*$A$4+D7*$A$6)</f>
+        <f t="shared" si="2"/>
         <v>0.39999999999999974</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C8" s="8">
         <v>0.36842105263157898</v>
       </c>
@@ -698,23 +707,23 @@
         <v>0.63157894736842102</v>
       </c>
       <c r="G8" s="8">
-        <f>C8*$A$2/(C8*$A$2+E8*$A$4+D8*$A$6)</f>
+        <f t="shared" si="0"/>
         <v>0.70000000000000007</v>
       </c>
       <c r="H8" s="8">
-        <f>D8*$A$6/(E8*$A$2+D8*$A$4+D8*$A$6)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I8" s="8">
-        <f>E8*$A$4/(C8*$A$2+E8*$A$4+D8*$A$6)</f>
+        <f t="shared" si="2"/>
         <v>0.29999999999999993</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C9" s="8">
         <v>0.5</v>
       </c>
@@ -726,23 +735,23 @@
         <v>0.5</v>
       </c>
       <c r="G9" s="8">
-        <f>C9*$A$2/(C9*$A$2+E9*$A$4+D9*$A$6)</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="H9" s="8">
-        <f>D9*$A$6/(E9*$A$2+D9*$A$4+D9*$A$6)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I9" s="8">
-        <f>E9*$A$4/(C9*$A$2+E9*$A$4+D9*$A$6)</f>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C10" s="8">
         <v>0.69230769230769196</v>
       </c>
@@ -753,23 +762,23 @@
         <v>0.30769230769230799</v>
       </c>
       <c r="G10" s="8">
-        <f>C10*$A$2/(C10*$A$2+E10*$A$4+D10*$A$6)</f>
+        <f t="shared" si="0"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="H10" s="8">
-        <f>D10*$A$6/(E10*$A$2+D10*$A$4+D10*$A$6)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I10" s="8">
-        <f>E10*$A$4/(C10*$A$2+E10*$A$4+D10*$A$6)</f>
+        <f t="shared" si="2"/>
         <v>0.10000000000000012</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -778,7 +787,7 @@
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C12" s="8">
         <v>2.8328611898017001E-2</v>
       </c>
@@ -805,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C13" s="8">
         <v>6.1919504643963001E-2</v>
       </c>
@@ -816,15 +825,15 @@
         <v>0.92879256965944301</v>
       </c>
       <c r="G13" s="8">
-        <f t="shared" ref="G13:G16" si="1">C13*$A$2/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
+        <f t="shared" ref="G13:G16" si="4">C13*$A$2/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
         <v>0.20000000000000079</v>
       </c>
       <c r="H13" s="8">
-        <f t="shared" ref="H13:H16" si="2">D13*$A$6/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
+        <f t="shared" ref="H13:H16" si="5">D13*$A$6/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
         <v>4.9999999999997775E-2</v>
       </c>
       <c r="I13" s="8">
-        <f t="shared" ref="I13:I16" si="3">E13*$A$4/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
+        <f t="shared" ref="I13:I16" si="6">E13*$A$4/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
         <v>0.75000000000000133</v>
       </c>
       <c r="K13">
@@ -832,7 +841,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C14" s="8">
         <v>0.102389078498294</v>
       </c>
@@ -843,15 +852,15 @@
         <v>0.88737201365187701</v>
       </c>
       <c r="G14" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.30000000000000154</v>
       </c>
       <c r="H14" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.9999999999998303E-2</v>
       </c>
       <c r="I14" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.65000000000000013</v>
       </c>
       <c r="K14">
@@ -859,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C15" s="8">
         <v>0.15209125475285201</v>
       </c>
@@ -870,15 +879,15 @@
         <v>0.83650190114068401</v>
       </c>
       <c r="G15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.40000000000000036</v>
       </c>
       <c r="H15" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5.0000000000000482E-2</v>
       </c>
       <c r="I15" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.54999999999999916</v>
       </c>
       <c r="K15">
@@ -886,7 +895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C16" s="8">
         <v>0.21459227467811201</v>
       </c>
@@ -897,15 +906,15 @@
         <v>0.77253218884120201</v>
       </c>
       <c r="G16" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.49999999999999978</v>
       </c>
       <c r="H16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5.0000000000001064E-2</v>
       </c>
       <c r="I16" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.44999999999999907</v>
       </c>
       <c r="K16">
@@ -913,7 +922,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C17" s="8">
         <v>0.25229357798165097</v>
       </c>
@@ -924,23 +933,23 @@
         <v>0.73394495412843996</v>
       </c>
       <c r="G17" s="8">
-        <f t="shared" ref="G17:G20" si="4">C17*$A$2/(C17*$A$2+E17*$A$4+D17*$A$6)</f>
+        <f t="shared" ref="G17:G20" si="7">C17*$A$2/(C17*$A$2+E17*$A$4+D17*$A$6)</f>
         <v>0.55000000000000027</v>
       </c>
       <c r="H17" s="8">
-        <f t="shared" ref="H17:H20" si="5">D17*$A$6/(C17*$A$2+E17*$A$4+D17*$A$6)</f>
+        <f t="shared" ref="H17:H20" si="8">D17*$A$6/(C17*$A$2+E17*$A$4+D17*$A$6)</f>
         <v>4.9999999999999163E-2</v>
       </c>
       <c r="I17" s="8">
-        <f t="shared" ref="I17:I20" si="6">E17*$A$4/(C17*$A$2+E17*$A$4+D17*$A$6)</f>
+        <f t="shared" ref="I17:I20" si="9">E17*$A$4/(C17*$A$2+E17*$A$4+D17*$A$6)</f>
         <v>0.40000000000000063</v>
       </c>
       <c r="K17">
-        <f t="shared" ref="K17:K20" si="7">SUM(G17:I17)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+        <f t="shared" ref="K17:K20" si="10">SUM(G17:I17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C18" s="8">
         <v>0.34574468085106402</v>
       </c>
@@ -951,23 +960,23 @@
         <v>0.63829787234042601</v>
       </c>
       <c r="G18" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.64999999999999925</v>
       </c>
       <c r="H18" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>5.0000000000001057E-2</v>
       </c>
       <c r="I18" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.29999999999999971</v>
       </c>
       <c r="K18">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C19" s="8">
         <v>0.474683544303797</v>
       </c>
@@ -978,23 +987,23 @@
         <v>0.506329113924051</v>
       </c>
       <c r="G19" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.74999999999999944</v>
       </c>
       <c r="H19" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>5.000000000000028E-2</v>
       </c>
       <c r="I19" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.20000000000000021</v>
       </c>
       <c r="K19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C20" s="8">
         <v>0.6640625</v>
       </c>
@@ -1005,19 +1014,19 @@
         <v>0.3125</v>
       </c>
       <c r="G20" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.85</v>
       </c>
       <c r="H20" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.05</v>
       </c>
       <c r="I20" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.1</v>
       </c>
       <c r="K20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finally added networking experiments
</commit_message>
<xml_diff>
--- a/transitions_to_real_P.xlsx
+++ b/transitions_to_real_P.xlsx
@@ -563,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:I13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -581,7 +581,9 @@
     <col min="8" max="8" width="10.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.140625" customWidth="1"/>
     <col min="10" max="10" width="4.140625" style="3" customWidth="1"/>
-    <col min="11" max="16" width="8.85546875" customWidth="1"/>
+    <col min="11" max="13" width="8.85546875" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.85546875" customWidth="1"/>
     <col min="17" max="17" width="26.5703125" customWidth="1"/>
     <col min="18" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
@@ -880,88 +882,88 @@
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="C13" s="8">
-        <v>0.317460317460317</v>
-      </c>
-      <c r="D13" s="8">
-        <v>4.7619047619047998E-2</v>
-      </c>
-      <c r="E13" s="8">
-        <v>0.634920634920635</v>
+      <c r="C13" s="13">
+        <v>0.29530000000000001</v>
+      </c>
+      <c r="D13" s="13">
+        <v>0.1171</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0.58760000000000001</v>
       </c>
       <c r="G13" s="9">
-        <f>C13*$A$2/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
-        <v>0.39999999999999891</v>
+        <f t="shared" ref="G13" si="11">C13*$A$2/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
+        <v>0.30150086784875607</v>
       </c>
       <c r="H13" s="9">
-        <f>D13*$A$6/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
-        <v>0.20000000000000137</v>
+        <f t="shared" ref="H13" si="12">D13*$A$6/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
+        <v>0.39852976210734092</v>
       </c>
       <c r="I13" s="9">
-        <f>E13*$A$4/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
-        <v>0.39999999999999958</v>
+        <f t="shared" ref="I13" si="13">E13*$A$4/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
+        <v>0.29996937004390289</v>
       </c>
       <c r="K13">
-        <f>SUM(G13:I13)</f>
+        <f t="shared" ref="K13" si="14">SUM(G13:I13)</f>
         <v>0.99999999999999989</v>
       </c>
       <c r="L13">
-        <f>G13*I13</f>
-        <v>0.15999999999999939</v>
+        <f t="shared" ref="L13" si="15">G13*I13</f>
+        <v>9.0441025396281377E-2</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="C14" s="8">
-        <v>0.32608695652173902</v>
+        <v>0.317460317460317</v>
       </c>
       <c r="D14" s="8">
-        <v>2.1739130434783E-2</v>
+        <v>4.7619047619047998E-2</v>
       </c>
       <c r="E14" s="8">
-        <v>0.65217391304347805</v>
+        <v>0.634920634920635</v>
       </c>
       <c r="G14" s="9">
         <f>C14*$A$2/(C14*$A$2+E14*$A$4+D14*$A$6)</f>
-        <v>0.44999999999999918</v>
+        <v>0.39999999999999891</v>
       </c>
       <c r="H14" s="9">
         <f>D14*$A$6/(C14*$A$2+E14*$A$4+D14*$A$6)</f>
-        <v>0.10000000000000164</v>
+        <v>0.20000000000000137</v>
       </c>
       <c r="I14" s="9">
         <f>E14*$A$4/(C14*$A$2+E14*$A$4+D14*$A$6)</f>
-        <v>0.44999999999999918</v>
+        <v>0.39999999999999958</v>
       </c>
       <c r="K14">
         <f>SUM(G14:I14)</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="L14">
         <f>G14*I14</f>
-        <v>0.20249999999999926</v>
+        <v>0.15999999999999939</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="C15" s="8">
-        <v>0.32986111111111099</v>
+        <v>0.32608695652173902</v>
       </c>
       <c r="D15" s="8">
-        <v>1.0416666666666999E-2</v>
+        <v>2.1739130434783E-2</v>
       </c>
       <c r="E15" s="8">
-        <v>0.65972222222222199</v>
+        <v>0.65217391304347805</v>
       </c>
       <c r="G15" s="9">
         <f>C15*$A$2/(C15*$A$2+E15*$A$4+D15*$A$6)</f>
-        <v>0.47499999999999926</v>
+        <v>0.44999999999999918</v>
       </c>
       <c r="H15" s="9">
         <f>D15*$A$6/(C15*$A$2+E15*$A$4+D15*$A$6)</f>
-        <v>5.0000000000001529E-2</v>
+        <v>0.10000000000000164</v>
       </c>
       <c r="I15" s="9">
         <f>E15*$A$4/(C15*$A$2+E15*$A$4+D15*$A$6)</f>
-        <v>0.47499999999999926</v>
+        <v>0.44999999999999918</v>
       </c>
       <c r="K15">
         <f>SUM(G15:I15)</f>
@@ -969,16 +971,39 @@
       </c>
       <c r="L15">
         <f>G15*I15</f>
+        <v>0.20249999999999926</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="C16" s="8">
+        <v>0.32986111111111099</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1.0416666666666999E-2</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.65972222222222199</v>
+      </c>
+      <c r="G16" s="9">
+        <f>C16*$A$2/(C16*$A$2+E16*$A$4+D16*$A$6)</f>
+        <v>0.47499999999999926</v>
+      </c>
+      <c r="H16" s="9">
+        <f>D16*$A$6/(C16*$A$2+E16*$A$4+D16*$A$6)</f>
+        <v>5.0000000000001529E-2</v>
+      </c>
+      <c r="I16" s="9">
+        <f>E16*$A$4/(C16*$A$2+E16*$A$4+D16*$A$6)</f>
+        <v>0.47499999999999926</v>
+      </c>
+      <c r="K16">
+        <f>SUM(G16:I16)</f>
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <f>G16*I16</f>
         <v>0.2256249999999993</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:17">
       <c r="C19" s="8"/>
@@ -997,50 +1022,70 @@
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:17">
-      <c r="C22" s="4" t="s">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="C23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I23" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
-      <c r="Q26" s="8">
+    <row r="27" spans="1:17">
+      <c r="Q27" s="8">
         <f>E12+D12</f>
         <v>0.72222222222222299</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
-      <c r="O27">
+    <row r="28" spans="1:17">
+      <c r="O28">
         <f>6971+365</f>
         <v>7336</v>
+      </c>
+    </row>
+    <row r="34" spans="14:14">
+      <c r="N34" s="8">
+        <f>D15+E15</f>
+        <v>0.67391304347826109</v>
+      </c>
+    </row>
+    <row r="37" spans="14:14">
+      <c r="N37">
+        <f>5876+1171</f>
+        <v>7047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added last network experiments
</commit_message>
<xml_diff>
--- a/transitions_to_real_P.xlsx
+++ b/transitions_to_real_P.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ingframin/BroadcastSimulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BroadcastSimulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C52898-15AE-ED40-8D63-112B68634CB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -69,12 +68,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000000000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -223,10 +222,10 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Excel Built-in 60% - Accent2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Excel Built-in Bad" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Excel Built-in Good" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Excel Built-in Note" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Excel Built-in 60% - Accent2" xfId="3"/>
+    <cellStyle name="Excel Built-in Bad" xfId="2"/>
+    <cellStyle name="Excel Built-in Good" xfId="4"/>
+    <cellStyle name="Excel Built-in Note" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -572,33 +571,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="2" max="2" width="3.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="3.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" customWidth="1"/>
-    <col min="10" max="10" width="4.1640625" style="3" customWidth="1"/>
-    <col min="11" max="13" width="8.83203125" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.83203125" customWidth="1"/>
-    <col min="17" max="17" width="26.5" customWidth="1"/>
-    <col min="18" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" style="3" customWidth="1"/>
+    <col min="11" max="13" width="8.85546875" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.85546875" customWidth="1"/>
+    <col min="17" max="17" width="26.42578125" customWidth="1"/>
+    <col min="18" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -631,7 +630,7 @@
         <v>0.11111111111111099</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>60</v>
       </c>
@@ -663,7 +662,7 @@
         <v>0.15999999999999992</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -695,7 +694,7 @@
         <v>0.20999999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>30</v>
       </c>
@@ -727,7 +726,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -757,9 +756,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C6" s="8">
         <v>0.42857142857142899</v>
@@ -787,7 +786,7 @@
         <v>0.23999999999999991</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18">
       <c r="C7" s="8">
         <v>0.53846153846153799</v>
       </c>
@@ -806,7 +805,7 @@
         <v>0.30000000000000043</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18">
       <c r="C8" s="8">
         <v>0.66666666666666696</v>
       </c>
@@ -824,7 +823,7 @@
         <v>0.19481460606304599</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18">
       <c r="C9" s="8">
         <v>0.81818181818181801</v>
       </c>
@@ -843,7 +842,7 @@
         <v>0.1000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18">
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -851,7 +850,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" s="10" customFormat="1">
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -860,100 +859,100 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18">
       <c r="C12" s="13">
-        <v>0.27777777777777801</v>
+        <v>0.26319999999999999</v>
       </c>
       <c r="D12" s="13">
-        <v>0.16666666666666699</v>
+        <v>0.21049999999999999</v>
       </c>
       <c r="E12" s="13">
-        <v>0.55555555555555602</v>
+        <v>0.52629999999999999</v>
       </c>
       <c r="G12" s="9">
         <f t="shared" ref="G12" si="6">C12*$A$2/(C12*$A$2+E12*$A$4+D12*$A$6)</f>
-        <v>0.24999999999999983</v>
+        <v>0.30005130056430618</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" ref="H12" si="7">D12*$A$6/(C12*$A$2+E12*$A$4+D12*$A$6)</f>
-        <v>0.50000000000000022</v>
+        <v>0.39995439949839451</v>
       </c>
       <c r="I12" s="9">
         <f t="shared" ref="I12" si="8">E12*$A$4/(C12*$A$2+E12*$A$4+D12*$A$6)</f>
-        <v>0.24999999999999983</v>
+        <v>0.29999429993729931</v>
       </c>
       <c r="K12">
         <f t="shared" ref="K12" si="9">SUM(G12:I12)</f>
-        <v>0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <f t="shared" ref="L12" si="10">G12*I12</f>
-        <v>6.2499999999999917E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>9.0013679858065215E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="C13" s="13">
-        <v>0.29530000000000001</v>
+        <v>0.30299999999999999</v>
       </c>
       <c r="D13" s="13">
-        <v>0.1171</v>
+        <v>9.0899999999999995E-2</v>
       </c>
       <c r="E13" s="13">
-        <v>0.58760000000000001</v>
+        <v>0.60609999999999997</v>
       </c>
       <c r="G13" s="9">
         <f t="shared" ref="G13" si="11">C13*$A$2/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
-        <v>0.30150086784875607</v>
+        <v>0.39997359910236946</v>
       </c>
       <c r="H13" s="9">
         <f t="shared" ref="H13" si="12">D13*$A$6/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
-        <v>0.39852976210734092</v>
+        <v>0.19998679955118473</v>
       </c>
       <c r="I13" s="9">
         <f t="shared" ref="I13" si="13">E13*$A$4/(C13*$A$2+E13*$A$4+D13*$A$6)</f>
-        <v>0.29996937004390289</v>
+        <v>0.40003960134644573</v>
       </c>
       <c r="K13">
         <f t="shared" ref="K13" si="14">SUM(G13:I13)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="L13">
         <f t="shared" ref="L13" si="15">G13*I13</f>
-        <v>9.0441025396281377E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>0.16000527913401499</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="C14" s="8">
-        <v>0.317460317460317</v>
+        <v>0.31909999999999999</v>
       </c>
       <c r="D14" s="8">
-        <v>4.7619047619047998E-2</v>
+        <v>4.2599999999999999E-2</v>
       </c>
       <c r="E14" s="8">
-        <v>0.634920634920635</v>
+        <v>0.63829999999999998</v>
       </c>
       <c r="G14" s="9">
         <f>C14*$A$2/(C14*$A$2+E14*$A$4+D14*$A$6)</f>
-        <v>0.39999999999999891</v>
+        <v>0.44991187874515337</v>
       </c>
       <c r="H14" s="9">
         <f>D14*$A$6/(C14*$A$2+E14*$A$4+D14*$A$6)</f>
-        <v>0.20000000000000137</v>
+        <v>0.100105745505816</v>
       </c>
       <c r="I14" s="9">
         <f>E14*$A$4/(C14*$A$2+E14*$A$4+D14*$A$6)</f>
-        <v>0.39999999999999958</v>
+        <v>0.44998237574903072</v>
       </c>
       <c r="K14">
         <f>SUM(G14:I14)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <f>G14*I14</f>
-        <v>0.15999999999999939</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+        <v>0.20245241607545394</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="C15" s="8">
         <v>0.32608695652173902</v>
       </c>
@@ -965,15 +964,15 @@
       </c>
       <c r="G15" s="9">
         <f>C15*$A$2/(C15*$A$2+E15*$A$4+D15*$A$6)</f>
-        <v>0.44999999999999918</v>
+        <v>0.47368421052631532</v>
       </c>
       <c r="H15" s="9">
         <f>D15*$A$6/(C15*$A$2+E15*$A$4+D15*$A$6)</f>
-        <v>0.10000000000000164</v>
+        <v>5.2631578947369334E-2</v>
       </c>
       <c r="I15" s="9">
         <f>E15*$A$4/(C15*$A$2+E15*$A$4+D15*$A$6)</f>
-        <v>0.44999999999999918</v>
+        <v>0.47368421052631532</v>
       </c>
       <c r="K15">
         <f>SUM(G15:I15)</f>
@@ -981,10 +980,10 @@
       </c>
       <c r="L15">
         <f>G15*I15</f>
-        <v>0.20249999999999926</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+        <v>0.22437673130193861</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="C16" s="8">
         <v>0.32986111111111099</v>
       </c>
@@ -996,15 +995,15 @@
       </c>
       <c r="G16" s="9">
         <f>C16*$A$2/(C16*$A$2+E16*$A$4+D16*$A$6)</f>
-        <v>0.47499999999999926</v>
+        <v>0.48717948717948678</v>
       </c>
       <c r="H16" s="9">
         <f>D16*$A$6/(C16*$A$2+E16*$A$4+D16*$A$6)</f>
-        <v>5.0000000000001529E-2</v>
+        <v>2.5641025641026445E-2</v>
       </c>
       <c r="I16" s="9">
         <f>E16*$A$4/(C16*$A$2+E16*$A$4+D16*$A$6)</f>
-        <v>0.47499999999999926</v>
+        <v>0.48717948717948678</v>
       </c>
       <c r="K16">
         <f>SUM(G16:I16)</f>
@@ -1012,10 +1011,10 @@
       </c>
       <c r="L16">
         <f>G16*I16</f>
-        <v>0.2256249999999993</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+        <v>0.23734385272846772</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1023,7 +1022,7 @@
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17">
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -1031,7 +1030,7 @@
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17">
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -1039,7 +1038,7 @@
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="14"/>
@@ -1054,7 +1053,7 @@
       <c r="L22" s="14"/>
       <c r="M22" s="14"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17">
       <c r="C23" s="4" t="s">
         <v>4</v>
       </c>
@@ -1073,26 +1072,36 @@
       <c r="I23" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q23" s="8">
+        <f>E12+D12</f>
+        <v>0.73680000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="D26" s="8">
+        <f>E13+D13</f>
+        <v>0.69699999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="Q27" s="8">
         <f>E12+D12</f>
-        <v>0.72222222222222299</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+        <v>0.73680000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="O28">
         <f>6971+365</f>
         <v>7336</v>
       </c>
     </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="14:14">
       <c r="N34" s="8">
         <f>D15+E15</f>
         <v>0.67391304347826109</v>
       </c>
     </row>
-    <row r="37" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="14:14">
       <c r="N37">
         <f>5876+1171</f>
         <v>7047</v>
@@ -1105,29 +1114,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC122C4E-863B-2A49-A795-0C5CF5293EA6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="3.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="3.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" customWidth="1"/>
-    <col min="10" max="10" width="4.1640625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1169,7 @@
         <v>0.11111111111111099</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>90</v>
       </c>
@@ -1170,7 +1179,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1181,7 +1190,7 @@
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>30</v>
       </c>
@@ -1192,7 +1201,7 @@
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1201,28 +1210,28 @@
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="8">
-        <f t="shared" ref="E2:E9" si="0">1-C5</f>
+        <f t="shared" ref="E5" si="0">1-C5</f>
         <v>0.75</v>
       </c>
       <c r="G5" s="9">
-        <f t="shared" ref="G2:G9" si="1">C5*$A$2/(C5*$A$2+E5*$A$4+D5*$A$6)</f>
+        <f t="shared" ref="G5" si="1">C5*$A$2/(C5*$A$2+E5*$A$4+D5*$A$6)</f>
         <v>0.5</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9">
-        <f t="shared" ref="I2:I9" si="2">E5*$A$4/(C5*$A$2+E5*$A$4+D5*$A$6)</f>
+        <f t="shared" ref="I5" si="2">E5*$A$4/(C5*$A$2+E5*$A$4+D5*$A$6)</f>
         <v>0.5</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K2:K6" si="3">SUM(G5:I5)</f>
+        <f t="shared" ref="K5" si="3">SUM(G5:I5)</f>
         <v>1</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L2:L6" si="4">G5*I5</f>
+        <f t="shared" ref="L5" si="4">G5*I5</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>200</v>
       </c>
@@ -1233,7 +1242,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18">
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -1241,7 +1250,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18">
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -1249,7 +1258,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18">
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -1257,7 +1266,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18">
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -1265,7 +1274,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" s="10" customFormat="1">
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -1274,7 +1283,7 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18">
       <c r="C12" s="13">
         <v>0.27777777777777801</v>
       </c>
@@ -1305,7 +1314,7 @@
         <v>7.4074074074074001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18">
       <c r="C13" s="13">
         <v>0.29530000000000001</v>
       </c>
@@ -1336,7 +1345,7 @@
         <v>0.10244586694729074</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18">
       <c r="C14" s="8">
         <v>0.317460317460317</v>
       </c>
@@ -1367,7 +1376,7 @@
         <v>0.16666666666666621</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18">
       <c r="C15" s="8">
         <v>0.32608695652173902</v>
       </c>
@@ -1398,7 +1407,7 @@
         <v>0.20241566014160703</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18">
       <c r="C16" s="8">
         <v>0.32986111111111099</v>
       </c>
@@ -1429,7 +1438,7 @@
         <v>0.22099785736149316</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17">
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1437,7 +1446,7 @@
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17">
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -1445,7 +1454,7 @@
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17">
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -1453,7 +1462,7 @@
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="14"/>
@@ -1468,7 +1477,7 @@
       <c r="L22" s="14"/>
       <c r="M22" s="14"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17">
       <c r="C23" s="4" t="s">
         <v>4</v>
       </c>
@@ -1488,25 +1497,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17">
       <c r="Q27" s="8">
         <f>E12+D12</f>
         <v>0.72222222222222299</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17">
       <c r="O28">
         <f>6971+365</f>
         <v>7336</v>
       </c>
     </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="14:14">
       <c r="N34" s="8">
         <f>D15+E15</f>
         <v>0.67391304347826109</v>
       </c>
     </row>
-    <row r="37" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="14:14">
       <c r="N37">
         <f>5876+1171</f>
         <v>7047</v>

</xml_diff>